<commit_message>
Minor documentation language edits.
</commit_message>
<xml_diff>
--- a/docs/Curation template column specification.xlsx
+++ b/docs/Curation template column specification.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\hipc-dashboard-pipeline\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="9947"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17960" windowHeight="8107"/>
   </bookViews>
   <sheets>
     <sheet name="shared" sheetId="5" r:id="rId1"/>
@@ -18,6 +13,7 @@
     <sheet name="pick lists" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <customWorkbookViews>
     <customWorkbookView name="Filter 1" guid="{9223F368-C2D9-494C-8931-FB9817D029AF}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
@@ -52,9 +48,6 @@
   </si>
   <si>
     <t>cohort</t>
-  </si>
-  <si>
-    <t>A mnemonic name describing the population where the immune signature is measured.</t>
   </si>
   <si>
     <t>free text</t>
@@ -1150,6 +1143,9 @@
       </rPr>
       <t xml:space="preserve"> ID of vaccine used.</t>
     </r>
+  </si>
+  <si>
+    <t>A short, descriptive name for the population where the immune signature is measured.</t>
   </si>
 </sst>
 </file>
@@ -1369,9 +1365,7 @@
   <dxfs count="22">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
+        <left/>
         <right style="thin">
           <color auto="1"/>
         </right>
@@ -1425,7 +1419,9 @@
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
         <right style="thin">
           <color auto="1"/>
         </right>
@@ -1754,11 +1750,11 @@
     <tableColumn id="2" name="exposure_process" dataDxfId="7"/>
     <tableColumn id="3" name="is_model" dataDxfId="6"/>
     <tableColumn id="4" name="method" dataDxfId="5"/>
-    <tableColumn id="5" name="route" dataDxfId="3"/>
-    <tableColumn id="6" name="response_behavior" dataDxfId="2"/>
-    <tableColumn id="7" name="response_behavior_type" dataDxfId="1"/>
-    <tableColumn id="8" name="time_point_units" dataDxfId="0"/>
-    <tableColumn id="9" name="tissue_type_term_id" dataDxfId="4"/>
+    <tableColumn id="5" name="route" dataDxfId="4"/>
+    <tableColumn id="6" name="response_behavior" dataDxfId="3"/>
+    <tableColumn id="7" name="response_behavior_type" dataDxfId="2"/>
+    <tableColumn id="8" name="time_point_units" dataDxfId="1"/>
+    <tableColumn id="9" name="tissue_type_term_id" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="pick lists-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1964,7 +1960,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <cols>
@@ -2029,13 +2027,13 @@
         <v>8</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -2062,16 +2060,16 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -2098,16 +2096,16 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="C5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -2134,16 +2132,16 @@
     </row>
     <row r="6" spans="1:26" ht="24.7" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -2170,16 +2168,16 @@
     </row>
     <row r="7" spans="1:26" ht="24.7" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -2206,16 +2204,16 @@
     </row>
     <row r="8" spans="1:26" ht="24.7" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -2242,16 +2240,16 @@
     </row>
     <row r="9" spans="1:26" ht="37" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -2278,16 +2276,16 @@
     </row>
     <row r="10" spans="1:26" ht="37" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -2314,16 +2312,16 @@
     </row>
     <row r="11" spans="1:26" ht="99" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -2350,16 +2348,16 @@
     </row>
     <row r="12" spans="1:26" ht="61.7" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="D12" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -2386,16 +2384,16 @@
     </row>
     <row r="13" spans="1:26" ht="24.7" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -2422,16 +2420,16 @@
     </row>
     <row r="14" spans="1:26" ht="61.7" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="C14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -2458,16 +2456,16 @@
     </row>
     <row r="15" spans="1:26" ht="148" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="C15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>50</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -2494,16 +2492,16 @@
     </row>
     <row r="16" spans="1:26" ht="37" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -2530,16 +2528,16 @@
     </row>
     <row r="17" spans="1:26" ht="24.7" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="C17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -2566,16 +2564,16 @@
     </row>
     <row r="18" spans="1:26" ht="24.7" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="C18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -2602,16 +2600,16 @@
     </row>
     <row r="19" spans="1:26" ht="24.7" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="C19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -2638,16 +2636,16 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A20" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -2674,16 +2672,16 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A21" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="C21" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -2710,16 +2708,16 @@
     </row>
     <row r="22" spans="1:26" ht="37" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -2746,16 +2744,16 @@
     </row>
     <row r="23" spans="1:26" ht="49.35" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -2782,16 +2780,16 @@
     </row>
     <row r="24" spans="1:26" ht="24.7" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="C24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>79</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -2860,16 +2858,16 @@
     </row>
     <row r="2" spans="1:26" ht="37" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>81</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -2896,16 +2894,16 @@
     </row>
     <row r="3" spans="1:26" ht="37" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>84</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -2932,16 +2930,16 @@
     </row>
     <row r="4" spans="1:26" ht="24.7" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>87</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -2968,16 +2966,16 @@
     </row>
     <row r="5" spans="1:26" ht="24.7" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -3004,16 +3002,16 @@
     </row>
     <row r="6" spans="1:26" ht="24.7" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>93</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -3079,16 +3077,16 @@
     </row>
     <row r="2" spans="1:26" ht="24.7" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -3115,16 +3113,16 @@
     </row>
     <row r="3" spans="1:26" ht="24.7" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -3151,16 +3149,16 @@
     </row>
     <row r="4" spans="1:26" ht="37" x14ac:dyDescent="0.4">
       <c r="A4" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -3187,16 +3185,16 @@
     </row>
     <row r="5" spans="1:26" ht="61.7" x14ac:dyDescent="0.4">
       <c r="A5" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -3223,16 +3221,16 @@
     </row>
     <row r="6" spans="1:26" ht="24.7" x14ac:dyDescent="0.4">
       <c r="A6" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>104</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>105</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -3259,16 +3257,16 @@
     </row>
     <row r="7" spans="1:26" ht="24.7" x14ac:dyDescent="0.4">
       <c r="A7" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>108</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -3295,16 +3293,16 @@
     </row>
     <row r="8" spans="1:26" ht="24.7" x14ac:dyDescent="0.4">
       <c r="A8" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>111</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -3331,16 +3329,16 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A9" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>114</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -3367,16 +3365,16 @@
     </row>
     <row r="10" spans="1:26" ht="24.7" x14ac:dyDescent="0.4">
       <c r="A10" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>117</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -3439,635 +3437,635 @@
   <sheetData>
     <row r="1" spans="1:9" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A2" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="G2" s="12" t="s">
         <v>123</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>124</v>
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
+      <c r="A3" s="12" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A3" s="12" t="s">
-        <v>126</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="E3" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="G3" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="H3" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I3" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="H3" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="I3" s="18" t="s">
+    </row>
+    <row r="4" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
+      <c r="A4" s="12" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4" s="12" t="s">
-        <v>133</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="13"/>
       <c r="D4" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="F4" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="G4" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="H4" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="I4" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="I4" s="18" t="s">
+    </row>
+    <row r="5" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
+      <c r="A5" s="12" t="s">
         <v>138</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A5" s="12" t="s">
-        <v>139</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="F5" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="G5" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="H5" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="I5" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="I5" s="18" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A6" s="13"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="F6" s="15" t="s">
         <v>146</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>147</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="F7" s="12" t="s">
         <v>150</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>151</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="18" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
       <c r="D8" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
       <c r="I8" s="18" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
       <c r="I9" s="18" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
       <c r="I10" s="18" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
       <c r="I11" s="18" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
       <c r="I12" s="18" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
       <c r="I13" s="18" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
       <c r="I14" s="18" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
       <c r="I15" s="18" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
       <c r="I16" s="18" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
       <c r="D17" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
       <c r="I17" s="18" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
       <c r="I18" s="18" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
       <c r="D19" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
       <c r="I19" s="18" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
       <c r="I20" s="18" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
       <c r="D21" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
       <c r="I21" s="18" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
       <c r="I22" s="18" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A23" s="12"/>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
       <c r="I23" s="18" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
       <c r="I24" s="18" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
       <c r="I25" s="18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A26" s="12"/>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
       <c r="D26" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
       <c r="H26" s="12"/>
       <c r="I26" s="18" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>
       <c r="I27" s="18" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
       <c r="I28" s="18" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
       <c r="H29" s="12"/>
       <c r="I29" s="18" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A30" s="12"/>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
       <c r="D30" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
       <c r="H30" s="12"/>
       <c r="I30" s="18" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A31" s="12"/>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
       <c r="D31" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
       <c r="I31" s="18" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A32" s="12"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
       <c r="D32" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
       <c r="G32" s="12"/>
       <c r="H32" s="12"/>
       <c r="I32" s="18" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A33" s="12"/>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
       <c r="D33" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
       <c r="G33" s="12"/>
       <c r="H33" s="12"/>
       <c r="I33" s="18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A34" s="12"/>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
       <c r="D34" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
       <c r="G34" s="12"/>
       <c r="H34" s="12"/>
       <c r="I34" s="18" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A35" s="12"/>
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
       <c r="D35" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
       <c r="I35" s="18" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A36" s="12"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
       <c r="D36" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
       <c r="I36" s="18" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A37" s="12"/>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
       <c r="D37" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
       <c r="I37" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.4">
@@ -4075,14 +4073,14 @@
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12"/>
       <c r="H38" s="12"/>
       <c r="I38" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.4">
@@ -4090,14 +4088,14 @@
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
       <c r="D39" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
       <c r="G39" s="12"/>
       <c r="H39" s="12"/>
       <c r="I39" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.4">
@@ -4105,14 +4103,14 @@
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
       <c r="D40" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
       <c r="G40" s="12"/>
       <c r="H40" s="12"/>
       <c r="I40" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.4">
@@ -4120,14 +4118,14 @@
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
       <c r="D41" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
       <c r="G41" s="12"/>
       <c r="H41" s="12"/>
       <c r="I41" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.4">
@@ -4135,14 +4133,14 @@
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
       <c r="D42" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E42" s="12"/>
       <c r="F42" s="12"/>
       <c r="G42" s="12"/>
       <c r="H42" s="12"/>
       <c r="I42" s="18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.4">
@@ -4150,14 +4148,14 @@
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
       <c r="D43" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
       <c r="H43" s="12"/>
       <c r="I43" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.4">
@@ -4165,14 +4163,14 @@
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
       <c r="D44" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
       <c r="H44" s="12"/>
       <c r="I44" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.4">
@@ -4180,7 +4178,7 @@
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
       <c r="D45" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
@@ -4193,7 +4191,7 @@
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
       <c r="D46" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E46" s="12"/>
       <c r="F46" s="12"/>
@@ -4206,7 +4204,7 @@
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
       <c r="D47" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
@@ -4219,7 +4217,7 @@
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
       <c r="D48" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E48" s="12"/>
       <c r="F48" s="12"/>
@@ -4232,7 +4230,7 @@
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
       <c r="D49" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
@@ -4245,7 +4243,7 @@
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
       <c r="D50" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E50" s="12"/>
       <c r="F50" s="12"/>
@@ -4258,7 +4256,7 @@
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
       <c r="D51" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E51" s="12"/>
       <c r="F51" s="12"/>
@@ -4271,7 +4269,7 @@
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
       <c r="D52" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
@@ -4284,7 +4282,7 @@
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
       <c r="D53" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E53" s="12"/>
       <c r="F53" s="12"/>
@@ -4297,7 +4295,7 @@
       <c r="B54" s="12"/>
       <c r="C54" s="12"/>
       <c r="D54" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E54" s="12"/>
       <c r="F54" s="12"/>
@@ -4310,7 +4308,7 @@
       <c r="B55" s="12"/>
       <c r="C55" s="12"/>
       <c r="D55" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E55" s="12"/>
       <c r="F55" s="12"/>
@@ -4323,7 +4321,7 @@
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
       <c r="D56" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E56" s="12"/>
       <c r="F56" s="12"/>
@@ -4336,7 +4334,7 @@
       <c r="B57" s="12"/>
       <c r="C57" s="12"/>
       <c r="D57" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E57" s="12"/>
       <c r="F57" s="12"/>
@@ -4349,7 +4347,7 @@
       <c r="B58" s="12"/>
       <c r="C58" s="12"/>
       <c r="D58" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E58" s="12"/>
       <c r="F58" s="12"/>
@@ -4362,7 +4360,7 @@
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
       <c r="D59" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E59" s="12"/>
       <c r="F59" s="12"/>
@@ -4375,7 +4373,7 @@
       <c r="B60" s="12"/>
       <c r="C60" s="12"/>
       <c r="D60" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E60" s="12"/>
       <c r="F60" s="12"/>
@@ -4388,7 +4386,7 @@
       <c r="B61" s="12"/>
       <c r="C61" s="12"/>
       <c r="D61" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E61" s="12"/>
       <c r="F61" s="12"/>

</xml_diff>